<commit_message>
Fixed Analysis for if player has as a King
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\GitHub\Ultimate-Texas-Holdem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spamt\Documents\Code\Github\Ultimate-Texas-Holdem\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12438"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -317,7 +317,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -501,6 +501,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -536,6 +553,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -690,25 +724,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AH106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="51" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.15625" customWidth="1"/>
+    <col min="3" max="3" width="11.83984375" customWidth="1"/>
+    <col min="4" max="4" width="11.26171875" customWidth="1"/>
+    <col min="5" max="5" width="10.83984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.578125" customWidth="1"/>
+    <col min="7" max="7" width="11.578125" customWidth="1"/>
+    <col min="9" max="9" width="9.15625" customWidth="1"/>
+    <col min="10" max="10" width="11.15625" customWidth="1"/>
+    <col min="11" max="11" width="10.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="51" width="3.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -731,7 +765,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -754,7 +788,7 @@
         <v>-6282135</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -777,16 +811,16 @@
         <v>-4228180</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="U9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="T10" t="s">
         <v>85</v>
       </c>
@@ -830,7 +864,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="U11" t="s">
         <v>87</v>
       </c>
@@ -874,7 +908,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -917,11 +951,11 @@
       <c r="U12" t="s">
         <v>88</v>
       </c>
-      <c r="V12" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="W12" s="6" t="s">
-        <v>90</v>
+      <c r="V12" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="W12" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="X12" s="4" t="s">
         <v>90</v>
@@ -955,7 +989,7 @@
       </c>
       <c r="AH12" s="3"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +1068,7 @@
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1111,7 +1145,7 @@
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1186,7 +1220,7 @@
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1259,7 +1293,7 @@
       <c r="AG16" s="3"/>
       <c r="AH16" s="3"/>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1330,7 +1364,7 @@
       <c r="AG17" s="3"/>
       <c r="AH17" s="3"/>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1399,7 +1433,7 @@
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1466,7 +1500,7 @@
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1531,7 +1565,7 @@
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1594,7 +1628,7 @@
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1655,7 +1689,7 @@
       <c r="AG22" s="3"/>
       <c r="AH22" s="3"/>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1714,7 +1748,7 @@
       <c r="AG23" s="3"/>
       <c r="AH23" s="3"/>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1755,7 +1789,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1796,7 +1830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1828,7 +1862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1860,7 +1894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1892,7 +1926,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1924,7 +1958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1956,7 +1990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1988,7 +2022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -2020,7 +2054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -2052,7 +2086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -2084,7 +2118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -2116,7 +2150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -2148,7 +2182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -2180,7 +2214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2212,7 +2246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -2244,7 +2278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -2276,7 +2310,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -2308,7 +2342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -2340,7 +2374,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2372,7 +2406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -2404,7 +2438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -2436,7 +2470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -2468,7 +2502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -2500,7 +2534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -2532,7 +2566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -2564,7 +2598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -2596,7 +2630,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -2628,7 +2662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -2660,7 +2694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -2692,7 +2726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -2724,7 +2758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -2756,7 +2790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -2788,7 +2822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -2820,7 +2854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -2849,7 +2883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -2878,7 +2912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -2907,7 +2941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -2936,7 +2970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -2962,7 +2996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -2988,7 +3022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>66</v>
       </c>
@@ -3014,7 +3048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -3040,7 +3074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -3066,7 +3100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -3092,7 +3126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -3121,7 +3155,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>71</v>
       </c>
@@ -3147,7 +3181,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>72</v>
       </c>
@@ -3173,7 +3207,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>73</v>
       </c>
@@ -3199,7 +3233,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -3225,7 +3259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -3251,7 +3285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -3277,7 +3311,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>77</v>
       </c>
@@ -3303,7 +3337,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>78</v>
       </c>
@@ -3316,7 +3350,7 @@
         <v>1852995</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -3329,7 +3363,7 @@
         <v>1746075</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -3342,7 +3376,7 @@
         <v>1637745</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -3355,7 +3389,7 @@
         <v>1536215</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -3368,7 +3402,7 @@
         <v>1441235</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>83</v>
       </c>
@@ -3380,7 +3414,7 @@
         <v>1208830</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>84</v>
       </c>
@@ -3392,79 +3426,79 @@
         <v>1173180</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>4</v>
       </c>
@@ -3481,7 +3515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>4</v>
       </c>
@@ -3498,7 +3532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>4</v>
       </c>
@@ -3515,7 +3549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>14</v>
       </c>
@@ -3532,7 +3566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>14</v>
       </c>

</xml_diff>